<commit_message>
runnable version(hp ok, but no thp)
</commit_message>
<xml_diff>
--- a/paper/figures/mmprofPerformance.xlsx
+++ b/paper/figures/mmprofPerformance.xlsx
@@ -1,32 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongpingliu/projects/mmprof/paper/figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\mmprof\paper\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4811B95-B4FC-2D4E-875E-AF37D67242C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EB67827-5BEE-4C5D-9ED8-D14A2E4C2E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -117,13 +110,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0_ "/>
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -135,10 +128,16 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -182,13 +181,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -200,6 +199,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,8 +259,10 @@
                 <a:lumOff val="35000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -435,19 +437,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="pct50">
+            <a:pattFill prst="wdDnDiag">
               <a:fgClr>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:fgClr>
               <a:bgClr>
                 <a:schemeClr val="bg1"/>
               </a:bgClr>
             </a:pattFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -622,19 +623,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="pct30">
+            <a:pattFill prst="dkUpDiag">
               <a:fgClr>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:fgClr>
               <a:bgClr>
                 <a:schemeClr val="bg1"/>
               </a:bgClr>
             </a:pattFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -720,70 +720,70 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>2.5272225590000001</c:v>
+                  <c:v>2.24671916</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4786776860000002</c:v>
+                  <c:v>2.400661157</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91554309619999996</c:v>
+                  <c:v>0.88826902230000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7289185319999998</c:v>
+                  <c:v>2.7219310779999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1475981150000001</c:v>
+                  <c:v>3.1210909139999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0185761210000002</c:v>
+                  <c:v>1.995448114</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2039453990000002</c:v>
+                  <c:v>3.1958100389999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1937791010000001</c:v>
+                  <c:v>1.144057433</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5906227720000001</c:v>
+                  <c:v>1.4107831129999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.161793372</c:v>
+                  <c:v>1.304550815</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.7377590920000001</c:v>
+                  <c:v>1.200209096</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.31157049</c:v>
+                  <c:v>1.085817918</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.1695618149999998</c:v>
+                  <c:v>1.202900995</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1074273520000002</c:v>
+                  <c:v>2.2077848200000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.7449038029999997</c:v>
+                  <c:v>4.2137741059999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.947614599</c:v>
+                  <c:v>1.6992146720000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.72903932</c:v>
+                  <c:v>1.74695383</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.4586997230000001</c:v>
+                  <c:v>2.4217916320000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.6567773130000001</c:v>
+                  <c:v>1.463641653</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1288702769999999</c:v>
+                  <c:v>2.1508928350000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1981506577172336</c:v>
+                  <c:v>1.8315108614490032</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3979450268599996</c:v>
+                  <c:v>1.9911151201150006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -844,7 +844,7 @@
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1691231808"/>
@@ -944,7 +944,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -971,12 +971,12 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1714579040"/>
@@ -1025,7 +1025,7 @@
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1062,13 +1062,13 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.25" r="0.25" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
   <c:userShapes r:id="rId3"/>
 </c:chartSpace>
@@ -1621,16 +1621,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>141828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>221240</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>141828</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1694,38 +1694,41 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="75000"/>
                   <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>3.59</a:t>
+            <a:t>                                       </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
+            <a:rPr lang="en-US" sz="1000">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="75000"/>
                   <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>   </a:t>
+            <a:t>4.21</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>                    4.17       4.74</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-US" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -1996,21 +1999,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="7" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.46484375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="25.9" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>22</v>
@@ -2022,7 +2025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2033,10 +2036,14 @@
         <v>1.1548556430000001</v>
       </c>
       <c r="D2" s="5">
-        <v>2.5272225590000001</v>
+        <v>2.24671916</v>
+      </c>
+      <c r="E2" s="1">
+        <f>D2/C2</f>
+        <v>1.9454545454388015</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2047,10 +2054,15 @@
         <v>1.211019504</v>
       </c>
       <c r="D3" s="5">
-        <v>2.4786776860000002</v>
-      </c>
+        <v>2.400661157</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E24" si="0">D3/C3</f>
+        <v>1.9823472281582675</v>
+      </c>
+      <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2061,10 +2073,14 @@
         <v>1.003564296</v>
       </c>
       <c r="D4" s="5">
-        <v>0.91554309619999996</v>
+        <v>0.88826902230000004</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88511421325016937</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2075,10 +2091,14 @@
         <v>1.2825154830000001</v>
       </c>
       <c r="D5" s="5">
-        <v>2.7289185319999998</v>
+        <v>2.7219310779999999</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1223377916912054</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2089,10 +2109,14 @@
         <v>2.1744352299999998</v>
       </c>
       <c r="D6" s="5">
-        <v>3.1475981150000001</v>
+        <v>3.1210909139999998</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4353570393540764</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2103,10 +2127,14 @@
         <v>1.847819893</v>
       </c>
       <c r="D7" s="5">
-        <v>2.0185761210000002</v>
+        <v>1.995448114</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.079893187403844</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2117,10 +2145,14 @@
         <v>1.2216472899999999</v>
       </c>
       <c r="D8" s="5">
-        <v>3.2039453990000002</v>
+        <v>3.1958100389999999</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6159842248739404</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2131,10 +2163,14 @@
         <v>1.1077444860000001</v>
       </c>
       <c r="D9" s="5">
-        <v>1.1937791010000001</v>
+        <v>1.144057433</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0327809774356214</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2145,10 +2181,14 @@
         <v>1.4102391510000001</v>
       </c>
       <c r="D10" s="5">
-        <v>3.5906227720000001</v>
+        <v>1.4107831129999999</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0003857232297189</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2159,10 +2199,14 @@
         <v>1.2846243589999999</v>
       </c>
       <c r="D11" s="5">
-        <v>1.161793372</v>
+        <v>1.304550815</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0155115040909792</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2173,10 +2217,14 @@
         <v>1.175715032</v>
       </c>
       <c r="D12" s="5">
-        <v>2.7377590920000001</v>
+        <v>1.200209096</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0208333340421218</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -2187,10 +2235,14 @@
         <v>1.039970925</v>
       </c>
       <c r="D13" s="5">
-        <v>1.31157049</v>
+        <v>1.085817918</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0440848795844941</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -2201,10 +2253,14 @@
         <v>1.1698431439999999</v>
       </c>
       <c r="D14" s="5">
-        <v>4.1695618149999998</v>
+        <v>1.202900995</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0282583619603622</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -2215,10 +2271,14 @@
         <v>1.7502030719999999</v>
       </c>
       <c r="D15" s="5">
-        <v>2.1074273520000002</v>
+        <v>2.2077848200000001</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2614449462010773</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2229,10 +2289,14 @@
         <v>3.0303028099999998</v>
       </c>
       <c r="D16" s="5">
-        <v>4.7449038029999997</v>
+        <v>4.2137741059999998</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3905455560726621</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -2243,10 +2307,14 @@
         <v>1.0630532479999999</v>
       </c>
       <c r="D17" s="5">
-        <v>1.947614599</v>
+        <v>1.6992146720000001</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5984285596199979</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -2257,10 +2325,14 @@
         <v>1.763024699</v>
       </c>
       <c r="D18" s="5">
-        <v>1.72903932</v>
+        <v>1.74695383</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.99088449015540425</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -2271,10 +2343,14 @@
         <v>1.2461985799999999</v>
       </c>
       <c r="D19" s="5">
-        <v>2.4586997230000001</v>
+        <v>2.4217916320000001</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.943343276799433</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -2285,10 +2361,14 @@
         <v>1.134380454</v>
       </c>
       <c r="D20" s="5">
-        <v>1.6567773130000001</v>
+        <v>1.463641653</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2902564107473595</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -2299,16 +2379,24 @@
         <v>1.198762552</v>
       </c>
       <c r="D21" s="8">
-        <v>2.1288702769999999</v>
+        <v>2.1508928350000001</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7942609496863895</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
+      <c r="E22" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2321,10 +2409,14 @@
       </c>
       <c r="D23" s="6">
         <f>GEOMEAN(D2:D21)</f>
-        <v>2.1981506577172336</v>
+        <v>1.8315108614490032</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3529328603530371</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2337,13 +2429,17 @@
       </c>
       <c r="D24" s="6">
         <f>AVERAGE(D2:D21)</f>
-        <v>2.3979450268599996</v>
+        <v>1.9911151201150006</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4086457482790267</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>